<commit_message>
presentation figures and finer time steps
</commit_message>
<xml_diff>
--- a/Data/drp/drp_ery_2.xlsx
+++ b/Data/drp/drp_ery_2.xlsx
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,46 +449,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <v>6</v>
       </c>
       <c r="L2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="M2">
         <v>6</v>
       </c>
       <c r="N2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="O2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -496,46 +496,46 @@
         <v>0.25</v>
       </c>
       <c r="B3">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K3">
         <v>5</v>
       </c>
       <c r="L3">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="M3">
         <v>6</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="O3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -543,46 +543,46 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4">
         <v>4</v>
       </c>
       <c r="J4">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M4">
         <v>6</v>
       </c>
       <c r="N4">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="O4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -590,43 +590,43 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="L5">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="M5">
         <v>6</v>
       </c>
       <c r="N5">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O5">
         <v>6</v>
@@ -637,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -649,31 +649,31 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
       <c r="L6">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="O6">
         <v>6</v>
@@ -684,43 +684,43 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
         <v>10</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>16</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>28</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="L7">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="M7">
         <v>5</v>
       </c>
       <c r="N7">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O7">
         <v>6</v>
@@ -731,43 +731,43 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>39</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>28</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
-        <v>9</v>
-      </c>
       <c r="M8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N8">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="O8">
         <v>6</v>
@@ -784,37 +784,37 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I9">
         <v>3</v>
       </c>
       <c r="J9">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K9">
         <v>3</v>
       </c>
       <c r="L9">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="O9">
         <v>6</v>
@@ -825,43 +825,43 @@
         <v>32</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>52</v>
-      </c>
       <c r="G10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I10">
         <v>3</v>
       </c>
       <c r="J10">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>3</v>
       </c>
       <c r="N10">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="O10">
         <v>6</v>

</xml_diff>